<commit_message>
Create dataAnalysis program Create MAE and MSE graph
</commit_message>
<xml_diff>
--- a/Metrics.xlsx
+++ b/Metrics.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/myrjus002_myuct_ac_za/Documents/Honors/Project/DL4NTP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{F1AB10D7-1213-F74B-A6C5-DC30905275F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0E6BF64-481C-2841-91D3-6A832AED0962}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{F1AB10D7-1213-F74B-A6C5-DC30905275F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E311978B-8E63-7C42-9A01-24AAA4ED8046}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FBDCC98E-B53B-5C40-AF9A-D807A96AE78D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{FBDCC98E-B53B-5C40-AF9A-D807A96AE78D}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Size" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Dataset Size'!$A$1:$I$16</definedName>
     <definedName name="ComputationalMetrics" localSheetId="0">'Dataset Size'!$A$1:$I$16</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{DD4E9E8F-E1DF-5447-8270-28ABF99BE650}" name="ComputationalMetrics" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/justin/OneDrive - University of Cape Town/Honors/Project/DL4NTP/ComputationalMetrics.csv" thousands=" " tab="0" comma="1">
+    <textPr sourceFile="/Users/justin/OneDrive - University of Cape Town/Honors/Project/DL4NTP/ComputationalMetrics.csv" thousands=" " tab="0" comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>dataset_size</t>
   </si>
@@ -86,6 +87,15 @@
   <si>
     <t>Simple LSTM Training</t>
   </si>
+  <si>
+    <t>Simple LSTM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bidirectional LSTM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stacked LSTM</t>
+  </si>
 </sst>
 </file>
 
@@ -100,7 +110,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,8 +123,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -131,16 +147,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1658,6 +1700,1299 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simple LSTM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.3032383203333264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9674971259999934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3514693516666636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.537996175999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.559719642999937</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A98C-6D4F-BF26-D90C24737D59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Bidirectional LSTM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.9456438323333303</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2259017143333262</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.7716182076666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.097613319666635</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.109150503999963</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-A98C-6D4F-BF26-D90C24737D59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Stacked LSTM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.8282231943333231</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.804901075666633</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.407642105999933</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.573541249333296</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.456242404999962</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-A98C-6D4F-BF26-D90C24737D59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="555508992"/>
+        <c:axId val="555549136"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="555508992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Dataset Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555549136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="555549136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555508992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simple LSTM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.24141923400000032</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2745266999998763E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9239980000001639E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11066177699999917</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17018872000000032</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DFD-5142-B05B-7F46AEB2BC3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Bidirectional LSTM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.34275045966666734</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8556344333332733E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0358048333330559E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15466000900000132</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66719293399999868</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1DFD-5142-B05B-7F46AEB2BC3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Stacked LSTM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.9712686393333344</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2109265666665636E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8156416333333829E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24436456299999035</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34605179933334762</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1DFD-5142-B05B-7F46AEB2BC3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="555508992"/>
+        <c:axId val="555549136"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="555508992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Dataset Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555549136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="555549136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555508992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -1732,6 +3067,80 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
@@ -2768,6 +4177,1038 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2829,6 +5270,85 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0978AEC6-48C3-2744-9672-E0879C254C34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52388FE5-A7B8-5245-9AC5-DF9804EEAC27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7707CCF-CA57-FF42-8B45-9AFF7604A7B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3154,8 +5674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07BD30E-5775-9C42-A67E-9CEE302E347C}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="H11" sqref="H10:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3640,4 +6160,649 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A4D33E-B674-9743-A9A6-C058B0650987}">
+  <dimension ref="A1:Q16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="3">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.42547693899999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.29836798400000197</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2.7065173649999998</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.32926379300000203</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5.6706208569999896</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.87419275500000204</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2000</v>
+      </c>
+      <c r="L2" s="7">
+        <f t="shared" ref="L2:Q2" si="0">AVERAGE(D2:D4)</f>
+        <v>3.3032383203333264</v>
+      </c>
+      <c r="M2" s="8">
+        <f t="shared" si="0"/>
+        <v>0.24141923400000032</v>
+      </c>
+      <c r="N2" s="7">
+        <f t="shared" si="0"/>
+        <v>3.9456438323333303</v>
+      </c>
+      <c r="O2" s="8">
+        <f t="shared" si="0"/>
+        <v>0.34275045966666734</v>
+      </c>
+      <c r="P2" s="7">
+        <f t="shared" si="0"/>
+        <v>7.8282231943333231</v>
+      </c>
+      <c r="Q2" s="8">
+        <f t="shared" si="0"/>
+        <v>0.9712686393333344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B3" s="3">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.376536722</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.19543507499999799</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4.0052395340000002</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.36515818800000199</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8.6901207959999898</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.91042716700000104</v>
+      </c>
+      <c r="K3" s="3">
+        <v>4000</v>
+      </c>
+      <c r="L3" s="7">
+        <f>AVERAGE(D5:D7)</f>
+        <v>4.9674971259999934</v>
+      </c>
+      <c r="M3" s="8">
+        <f t="shared" ref="M3:Q3" si="1">AVERAGE(E5:E7)</f>
+        <v>5.2745266999998763E-2</v>
+      </c>
+      <c r="N3" s="7">
+        <f t="shared" si="1"/>
+        <v>7.2259017143333262</v>
+      </c>
+      <c r="O3" s="8">
+        <f t="shared" si="1"/>
+        <v>5.8556344333332733E-2</v>
+      </c>
+      <c r="P3" s="7">
+        <f t="shared" si="1"/>
+        <v>11.804901075666633</v>
+      </c>
+      <c r="Q3" s="8">
+        <f t="shared" si="1"/>
+        <v>6.2109265666665636E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B4" s="3">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4.1077012999999898</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.23045464300000101</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5.1251745979999903</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.333829397999998</v>
+      </c>
+      <c r="H4" s="2">
+        <v>9.12392792999999</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.1291859959999999</v>
+      </c>
+      <c r="K4" s="3">
+        <v>8000</v>
+      </c>
+      <c r="L4" s="7">
+        <f>AVERAGE(D8:D10)</f>
+        <v>8.3514693516666636</v>
+      </c>
+      <c r="M4" s="8">
+        <f t="shared" ref="M4:Q4" si="2">AVERAGE(E8:E10)</f>
+        <v>7.9239980000001639E-2</v>
+      </c>
+      <c r="N4" s="7">
+        <f t="shared" si="2"/>
+        <v>10.7716182076666</v>
+      </c>
+      <c r="O4" s="8">
+        <f t="shared" si="2"/>
+        <v>8.0358048333330559E-2</v>
+      </c>
+      <c r="P4" s="7">
+        <f t="shared" si="2"/>
+        <v>17.407642105999933</v>
+      </c>
+      <c r="Q4" s="8">
+        <f t="shared" si="2"/>
+        <v>9.8156416333333829E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4000</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3.2842889769999899</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.4299020999998497E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.71649289699999</v>
+      </c>
+      <c r="G5" s="2">
+        <v>6.1108578000002398E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>8.8239389639999999</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6.1757454999998601E-2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>16000</v>
+      </c>
+      <c r="L5" s="7">
+        <f>AVERAGE(D11:D13)</f>
+        <v>23.537996175999996</v>
+      </c>
+      <c r="M5" s="8">
+        <f t="shared" ref="M5:Q5" si="3">AVERAGE(E11:E13)</f>
+        <v>0.11066177699999917</v>
+      </c>
+      <c r="N5" s="7">
+        <f t="shared" si="3"/>
+        <v>25.097613319666635</v>
+      </c>
+      <c r="O5" s="8">
+        <f t="shared" si="3"/>
+        <v>0.15466000900000132</v>
+      </c>
+      <c r="P5" s="7">
+        <f t="shared" si="3"/>
+        <v>35.573541249333296</v>
+      </c>
+      <c r="Q5" s="8">
+        <f t="shared" si="3"/>
+        <v>0.24436456299999035</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>4000</v>
+      </c>
+      <c r="B6" s="3">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5.1347941689999903</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.29148080000005E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5.8929337629999896</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5.8193613999996702E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>11.997573824</v>
+      </c>
+      <c r="I6" s="2">
+        <v>6.2318996999998398E-2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>32000</v>
+      </c>
+      <c r="L6" s="7">
+        <f>AVERAGE(D14:D16)</f>
+        <v>27.559719642999937</v>
+      </c>
+      <c r="M6" s="8">
+        <f t="shared" ref="M6:Q6" si="4">AVERAGE(E14:E16)</f>
+        <v>0.17018872000000032</v>
+      </c>
+      <c r="N6" s="7">
+        <f t="shared" si="4"/>
+        <v>36.109150503999963</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" si="4"/>
+        <v>0.66719293399999868</v>
+      </c>
+      <c r="P6" s="7">
+        <f t="shared" si="4"/>
+        <v>61.456242404999962</v>
+      </c>
+      <c r="Q6" s="8">
+        <f t="shared" si="4"/>
+        <v>0.34605179933334762</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>4000</v>
+      </c>
+      <c r="B7" s="3">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6.4834082320000004</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5.10219719999973E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>12.068278483</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5.6366840999999099E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>14.593190438999899</v>
+      </c>
+      <c r="I7" s="2">
+        <v>6.2251344999999902E-2</v>
+      </c>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>8000</v>
+      </c>
+      <c r="B8" s="3">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.5612495729999898</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6.6389647000001106E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5.3990009849999998</v>
+      </c>
+      <c r="G8" s="2">
+        <v>7.0829722999995598E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>10.278124267999999</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.10733288599999399</v>
+      </c>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>8000</v>
+      </c>
+      <c r="B9" s="3">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7.7000585770000001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6.6008408000001795E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>11.740541104999901</v>
+      </c>
+      <c r="G9" s="2">
+        <v>9.8216536999998993E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>18.2345535349999</v>
+      </c>
+      <c r="I9" s="2">
+        <v>8.8901047000007297E-2</v>
+      </c>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>8000</v>
+      </c>
+      <c r="B10" s="3">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>12.793099905</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.105321885000002</v>
+      </c>
+      <c r="F10" s="2">
+        <v>15.1753125329999</v>
+      </c>
+      <c r="G10" s="2">
+        <v>7.2027884999997099E-2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>23.7102485149999</v>
+      </c>
+      <c r="I10" s="2">
+        <v>9.8235316000000197E-2</v>
+      </c>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>16000</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7.0387955790000003</v>
+      </c>
+      <c r="E11" s="2">
+        <v>9.7691435000001506E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>9.7152473300000004</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.10347123200000299</v>
+      </c>
+      <c r="H11" s="2">
+        <v>25.151644315999999</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.431100551</v>
+      </c>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>16000</v>
+      </c>
+      <c r="B12" s="3">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>21.658888183999998</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.109899661</v>
+      </c>
+      <c r="F12" s="2">
+        <v>22.920682683999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.187293181000001</v>
+      </c>
+      <c r="H12" s="2">
+        <v>34.754027811999897</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.149365174999985</v>
+      </c>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>16000</v>
+      </c>
+      <c r="B13" s="3">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>41.916304765</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.124394234999996</v>
+      </c>
+      <c r="F13" s="2">
+        <v>42.656909944999903</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.17321561399999999</v>
+      </c>
+      <c r="H13" s="2">
+        <v>46.814951620000002</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.15262796299998599</v>
+      </c>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>32000</v>
+      </c>
+      <c r="B14" s="3">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>14.642504319</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.16512470199999901</v>
+      </c>
+      <c r="F14" s="2">
+        <v>19.35722402</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.58452520299999799</v>
+      </c>
+      <c r="H14" s="2">
+        <v>37.182260513999999</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.402763028999999</v>
+      </c>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>32000</v>
+      </c>
+      <c r="B15" s="3">
+        <v>20</v>
+      </c>
+      <c r="C15" s="5">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>27.559569486999901</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.172136497000003</v>
+      </c>
+      <c r="F15" s="2">
+        <v>36.029147479999899</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.86313815399999705</v>
+      </c>
+      <c r="H15" s="2">
+        <v>59.468460385999997</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.33427033400002398</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>32000</v>
+      </c>
+      <c r="B16" s="3">
+        <v>30</v>
+      </c>
+      <c r="C16" s="5">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>40.477085122999902</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.17330496099999901</v>
+      </c>
+      <c r="F16" s="2">
+        <v>52.941080012</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.55391544500000101</v>
+      </c>
+      <c r="H16" s="2">
+        <v>87.718006314999897</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.30112203500001999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>